<commit_message>
ni idea d que he hecho
doc d P3, doc d P4, informe P4 y cambios en P4 como la nueva funcion y poco mas
</commit_message>
<xml_diff>
--- a/Practica_4/Pruebas.xlsx
+++ b/Practica_4/Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COSAS IMPORTANTES\cursos\CURSO 2024-2025\2 Cuatri\ESTRUCTURAS\Practicas_Estructuras\Practica_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294B487E-E81E-4E90-9898-A5C039FB41B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BAD22E-6529-4C0F-9C09-2DABF094560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F0C7F6E1-7056-4E60-A746-7098AFC46100}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tamaño de la lista</t>
   </si>
@@ -47,7 +47,10 @@
     <t>Particion (ms)</t>
   </si>
   <si>
-    <t>SeleccionInversaMultiple (ms)</t>
+    <t>SeleccionInversaMultiple V1 (ms)</t>
+  </si>
+  <si>
+    <t>SeleccionInversaMultiple V2 (ms)</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -121,30 +124,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -159,7 +276,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -167,12 +284,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -203,9 +316,7 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -276,7 +387,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -301,7 +411,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -316,7 +426,95 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -434,10 +632,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$300</c:f>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="299"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -484,34 +682,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>212</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>354</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>734</c:v>
+                  <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>970</c:v>
+                  <c:v>971</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1293</c:v>
+                  <c:v>1321</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1639</c:v>
+                  <c:v>1659</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2053</c:v>
+                  <c:v>2038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -524,7 +722,7 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -532,7 +730,124 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SeleccionInversaMultiple (ms)</c:v>
+                  <c:v>SeleccionInversaMultiple V1 (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>966</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1806</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2272</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2947</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0568-42EC-A9C1-1E6BE30DB304}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SeleccionInversaMultiple V2 (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -549,9 +864,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$12</c:f>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -559,34 +874,76 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>346</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>695</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>742</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1005</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1376</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1854</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2281</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2944</c:v>
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,16 +951,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F368-4FAE-A654-E8BEAE3465F6}"/>
+              <c16:uniqueId val="{00000002-0568-42EC-A9C1-1E6BE30DB304}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$D$1</c:f>
+              <c:f>Hoja1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -615,7 +972,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -624,9 +981,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$12</c:f>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -634,34 +991,76 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>413</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>706</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1018</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1486</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2716</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2639</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3530</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4140</c:v>
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>984</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2609</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3422</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -669,7 +1068,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C427-41BE-A691-0630A5585F6C}"/>
+              <c16:uniqueId val="{00000003-0568-42EC-A9C1-1E6BE30DB304}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1435,16 +1834,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>293370</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1473,16 +1872,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{51D99A94-49AF-42E8-9271-A42ACF218C57}" name="Tabla1" displayName="Tabla1" ref="A1:D12" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D12" xr:uid="{51D99A94-49AF-42E8-9271-A42ACF218C57}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{51D99A94-49AF-42E8-9271-A42ACF218C57}" name="Tabla1" displayName="Tabla1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:E12" xr:uid="{51D99A94-49AF-42E8-9271-A42ACF218C57}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
     <sortCondition ref="A1:A11"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8082C113-F345-4E22-B1E4-57A23B0F77F0}" name="Tamaño de la lista" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0863CB4B-4BA9-43B1-874C-3A6CF8416994}" name="SeleccionMultiple (ms)" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{666D8902-5E95-4389-886B-BBA8ACAC20B0}" name="SeleccionInversaMultiple (ms)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CFA97098-9E47-4142-8932-8C7ADD075303}" name="Particion (ms)" dataDxfId="0"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8082C113-F345-4E22-B1E4-57A23B0F77F0}" name="Tamaño de la lista" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0863CB4B-4BA9-43B1-874C-3A6CF8416994}" name="SeleccionMultiple (ms)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{47D0855B-79FC-43E3-9D46-D34F6E94EB50}" name="SeleccionInversaMultiple V1 (ms)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{666D8902-5E95-4389-886B-BBA8ACAC20B0}" name="SeleccionInversaMultiple V2 (ms)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CFA97098-9E47-4142-8932-8C7ADD075303}" name="Particion (ms)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1805,36 +2205,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A824FF81-A7F3-428F-9590-3F8EB4055A25}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -1846,146 +2250,179 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>10000</v>
       </c>
       <c r="B3" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>20000</v>
       </c>
       <c r="B4" s="1">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1">
-        <v>175</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="7">
+        <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>30000</v>
       </c>
       <c r="B5" s="1">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1">
-        <v>346</v>
+        <v>238</v>
       </c>
       <c r="D5" s="1">
-        <v>413</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="E5" s="7">
+        <v>391</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>40000</v>
       </c>
       <c r="B6" s="1">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="C6" s="1">
-        <v>695</v>
+        <v>449</v>
       </c>
       <c r="D6" s="1">
-        <v>706</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="7">
+        <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>50000</v>
       </c>
       <c r="B7" s="1">
         <v>496</v>
       </c>
       <c r="C7" s="1">
-        <v>742</v>
+        <v>716</v>
       </c>
       <c r="D7" s="1">
-        <v>1018</v>
+        <v>41</v>
+      </c>
+      <c r="E7" s="7">
+        <v>984</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>60000</v>
       </c>
       <c r="B8" s="1">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="C8" s="1">
-        <v>1005</v>
+        <v>966</v>
       </c>
       <c r="D8" s="1">
-        <v>1486</v>
+        <v>59</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1477</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>70000</v>
       </c>
       <c r="B9" s="1">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C9" s="1">
-        <v>1376</v>
+        <v>1362</v>
       </c>
       <c r="D9" s="1">
-        <v>2716</v>
+        <v>83</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1996</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>80000</v>
       </c>
       <c r="B10" s="1">
-        <v>1293</v>
+        <v>1321</v>
       </c>
       <c r="C10" s="1">
-        <v>1854</v>
+        <v>1806</v>
       </c>
       <c r="D10" s="1">
-        <v>2639</v>
+        <v>109</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2609</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>90000</v>
       </c>
       <c r="B11" s="1">
-        <v>1639</v>
+        <v>1659</v>
       </c>
       <c r="C11" s="1">
-        <v>2281</v>
+        <v>2272</v>
       </c>
       <c r="D11" s="1">
-        <v>3530</v>
+        <v>134</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3422</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>100000</v>
       </c>
-      <c r="B12" s="4">
-        <v>2053</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2944</v>
-      </c>
-      <c r="D12" s="4">
-        <v>4140</v>
+      <c r="B12" s="9">
+        <v>2038</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2947</v>
+      </c>
+      <c r="D12" s="9">
+        <v>167</v>
+      </c>
+      <c r="E12" s="10">
+        <v>4123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>